<commit_message>
Cập nhật tính năng mới
</commit_message>
<xml_diff>
--- a/report_monthly.xlsx
+++ b/report_monthly.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet 0" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,98 +436,47 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>AgeRange</t>
+          <t>Gender</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>ID</t>
+          <t>Customer ID</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>20-30</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>64828</v>
+        <v>2398</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>31-40</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1447731</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>41-50</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>3256151</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>51-60</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>3536658</v>
+        <v>5105</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>61-70</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>2713487</v>
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Phân tích / Nhận xét</t>
+        </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>71-80</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>1437292</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>80+</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>50308</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="inlineStr">
-        <is>
-          <t>Phân tích / Nhận xét</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Here's a report summarizing the data from the bar chart:
-The bar chart displays the distribution of IDs across various age groups. The '51-60' age group has the highest number of IDs at approximately 3.6 million, followed by the '41-50' group. The '61-70' age group has slightly fewer IDs. The '31-40' and '71-80' groups have a moderate number of IDs. The '20-30' and '80+' age groups have the lowest number of IDs. This suggests a concentration of IDs within the middle-age ranges.
-</t>
+          <t>Here's a brief report based on the pie chart:
+The pie chart displays the gender distribution of customers.  Males constitute a larger portion of the customer base at 68%, while females represent 32%. This suggests the product/service might be more appealing or marketed more effectively towards men.  Further investigation into customer demographics and marketing strategies could reveal opportunities for better engaging the female demographic.</t>
         </is>
       </c>
     </row>

</xml_diff>